<commit_message>
Updated master tables data
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/device_master.xlsx
+++ b/mosip_master/xlsx/device_master.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Desktop\NIRA MASTERDATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8655141A-1F73-4947-87DD-E2C23B37D328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C858CEA3-174C-4A7C-B1ED-AE78AACE540F}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="device_master" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -85,13 +80,16 @@
     <t>eng</t>
   </si>
   <si>
-    <t>t</t>
+    <t>true</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>f</t>
+    <t>2024-02-15 06:37:20.005</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
   <si>
     <t>Mock FingerPrint Scanner</t>
@@ -106,9 +104,18 @@
     <t>RealScan-G10</t>
   </si>
   <si>
+    <t>2025-12-30 21:00:00.000</t>
+  </si>
+  <si>
     <t>globaladmin</t>
   </si>
   <si>
+    <t>2024-04-09 14:51:54.264</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:11:40.050</t>
+  </si>
+  <si>
     <t>a8bcbb3a-93b3-41db-a6d7-0294618fb833</t>
   </si>
   <si>
@@ -118,6 +125,12 @@
     <t>DF0052000024031A</t>
   </si>
   <si>
+    <t>2024-04-09 14:49:58.336</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:12:13.846</t>
+  </si>
+  <si>
     <t>59c43c89-ff00-4041-a933-6d9603e1c331</t>
   </si>
   <si>
@@ -127,558 +140,97 @@
     <t>1FE4516</t>
   </si>
   <si>
+    <t>2024-04-09 14:47:52.426</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:12:32.057</t>
+  </si>
+  <si>
     <t>807b28a8-80cd-47e7-9258-71be5b81f0de</t>
   </si>
   <si>
     <t>UGA</t>
   </si>
   <si>
+    <t>2024-08-08 07:10:49.767</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:10:59.964</t>
+  </si>
+  <si>
     <t>ec48fb6e-1916-4124-bf4a-02f3bbb2f5d1</t>
   </si>
   <si>
     <t>DF0052000020940A</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:53:01.343</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:53:08.806</t>
+  </si>
+  <si>
+    <t>7f8de61a-3e80-42bd-9bf9-374049606439</t>
+  </si>
+  <si>
+    <t>TECHNO-531</t>
+  </si>
+  <si>
+    <t>srbgrb</t>
+  </si>
+  <si>
+    <t>2047-12-30 18:30:00.000</t>
+  </si>
+  <si>
+    <t>2024-08-29 12:42:17.042</t>
+  </si>
+  <si>
+    <t>2024-08-29 12:43:02.606</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -693,44 +245,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -758,31 +310,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -810,23 +345,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -838,174 +356,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EED699B-FD57-42DC-9B0A-D82EBD2217AF}">
-  <dimension ref="A1:Q42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1089,14 +616,14 @@
       <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="1">
-        <v>45337.275925995367</v>
+      <c r="M2" t="s">
+        <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1127,14 +654,14 @@
       <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1">
-        <v>45337.275925995367</v>
+      <c r="M3" t="s">
+        <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1165,14 +692,14 @@
       <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="1">
-        <v>45337.275925995367</v>
+      <c r="M4" t="s">
+        <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1203,14 +730,14 @@
       <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="1">
-        <v>45337.275925995367</v>
+      <c r="M5" t="s">
+        <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1241,14 +768,14 @@
       <c r="L6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="1">
-        <v>45337.275925995367</v>
+      <c r="M6" t="s">
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1279,14 +806,14 @@
       <c r="L7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="1">
-        <v>45337.275925995367</v>
+      <c r="M7" t="s">
+        <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1317,14 +844,14 @@
       <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="1">
-        <v>45337.275925995367</v>
+      <c r="M8" t="s">
+        <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1355,14 +882,14 @@
       <c r="L9" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="1">
-        <v>45337.275925995367</v>
+      <c r="M9" t="s">
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1393,14 +920,14 @@
       <c r="L10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="1">
-        <v>45337.275925995367</v>
+      <c r="M10" t="s">
+        <v>23</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1431,14 +958,14 @@
       <c r="L11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="1">
-        <v>45337.275925995367</v>
+      <c r="M11" t="s">
+        <v>23</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1469,14 +996,14 @@
       <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="1">
-        <v>45337.275925995367</v>
+      <c r="M12" t="s">
+        <v>23</v>
       </c>
       <c r="P12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1507,19 +1034,19 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="1">
-        <v>45337.275925995367</v>
+      <c r="M13" t="s">
+        <v>23</v>
       </c>
       <c r="P13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>2001</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -1545,19 +1072,19 @@
       <c r="L14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="1">
-        <v>45337.275925995367</v>
+      <c r="M14" t="s">
+        <v>23</v>
       </c>
       <c r="P14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>2002</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1583,19 +1110,19 @@
       <c r="L15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="1">
-        <v>45337.275925995367</v>
+      <c r="M15" t="s">
+        <v>23</v>
       </c>
       <c r="P15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>2003</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -1621,19 +1148,19 @@
       <c r="L16" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="1">
-        <v>45337.275925995367</v>
+      <c r="M16" t="s">
+        <v>23</v>
       </c>
       <c r="P16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>2004</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1659,19 +1186,19 @@
       <c r="L17" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="1">
-        <v>45337.275925995367</v>
+      <c r="M17" t="s">
+        <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>2005</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1697,19 +1224,19 @@
       <c r="L18" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="1">
-        <v>45337.275925995367</v>
+      <c r="M18" t="s">
+        <v>23</v>
       </c>
       <c r="P18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>2006</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -1735,19 +1262,19 @@
       <c r="L19" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="1">
-        <v>45337.275925995367</v>
+      <c r="M19" t="s">
+        <v>23</v>
       </c>
       <c r="P19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>2007</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -1773,19 +1300,19 @@
       <c r="L20" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="1">
-        <v>45337.275925995367</v>
+      <c r="M20" t="s">
+        <v>23</v>
       </c>
       <c r="P20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>2008</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -1811,19 +1338,19 @@
       <c r="L21" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="1">
-        <v>45337.275925995367</v>
+      <c r="M21" t="s">
+        <v>23</v>
       </c>
       <c r="P21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>2009</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -1849,19 +1376,19 @@
       <c r="L22" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="1">
-        <v>45337.275925995367</v>
+      <c r="M22" t="s">
+        <v>23</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>2010</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -1887,19 +1414,19 @@
       <c r="L23" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="1">
-        <v>45337.275925995367</v>
+      <c r="M23" t="s">
+        <v>23</v>
       </c>
       <c r="P23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>2011</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -1925,19 +1452,19 @@
       <c r="L24" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="1">
-        <v>45337.275925995367</v>
+      <c r="M24" t="s">
+        <v>23</v>
       </c>
       <c r="P24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>2012</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -1963,19 +1490,19 @@
       <c r="L25" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="1">
-        <v>45337.275925995367</v>
+      <c r="M25" t="s">
+        <v>23</v>
       </c>
       <c r="P25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>3001</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -2001,19 +1528,19 @@
       <c r="L26" t="s">
         <v>22</v>
       </c>
-      <c r="M26" s="1">
-        <v>45337.275925995367</v>
+      <c r="M26" t="s">
+        <v>23</v>
       </c>
       <c r="P26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>3002</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -2039,19 +1566,19 @@
       <c r="L27" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="1">
-        <v>45337.275925995367</v>
+      <c r="M27" t="s">
+        <v>23</v>
       </c>
       <c r="P27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>3003</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -2077,19 +1604,19 @@
       <c r="L28" t="s">
         <v>22</v>
       </c>
-      <c r="M28" s="1">
-        <v>45337.275925995367</v>
+      <c r="M28" t="s">
+        <v>23</v>
       </c>
       <c r="P28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>3004</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -2115,19 +1642,19 @@
       <c r="L29" t="s">
         <v>22</v>
       </c>
-      <c r="M29" s="1">
-        <v>45337.275925995367</v>
+      <c r="M29" t="s">
+        <v>23</v>
       </c>
       <c r="P29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>3005</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -2153,19 +1680,19 @@
       <c r="L30" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="1">
-        <v>45337.275925995367</v>
+      <c r="M30" t="s">
+        <v>23</v>
       </c>
       <c r="P30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>3006</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -2191,19 +1718,19 @@
       <c r="L31" t="s">
         <v>22</v>
       </c>
-      <c r="M31" s="1">
-        <v>45337.275925995367</v>
+      <c r="M31" t="s">
+        <v>23</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>3007</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -2229,19 +1756,19 @@
       <c r="L32" t="s">
         <v>22</v>
       </c>
-      <c r="M32" s="1">
-        <v>45337.275925995367</v>
+      <c r="M32" t="s">
+        <v>23</v>
       </c>
       <c r="P32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>3008</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
@@ -2267,19 +1794,19 @@
       <c r="L33" t="s">
         <v>22</v>
       </c>
-      <c r="M33" s="1">
-        <v>45337.275925995367</v>
+      <c r="M33" t="s">
+        <v>23</v>
       </c>
       <c r="P33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>3009</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
@@ -2305,19 +1832,19 @@
       <c r="L34" t="s">
         <v>22</v>
       </c>
-      <c r="M34" s="1">
-        <v>45337.275925995367</v>
+      <c r="M34" t="s">
+        <v>23</v>
       </c>
       <c r="P34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>3010</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
@@ -2343,19 +1870,19 @@
       <c r="L35" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="1">
-        <v>45337.275925995367</v>
+      <c r="M35" t="s">
+        <v>23</v>
       </c>
       <c r="P35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>3011</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
@@ -2381,19 +1908,19 @@
       <c r="L36" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="1">
-        <v>45337.275925995367</v>
+      <c r="M36" t="s">
+        <v>23</v>
       </c>
       <c r="P36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>3012</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -2419,19 +1946,19 @@
       <c r="L37" t="s">
         <v>22</v>
       </c>
-      <c r="M37" s="1">
-        <v>45337.275925995367</v>
+      <c r="M37" t="s">
+        <v>23</v>
       </c>
       <c r="P37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38">
         <v>939541443</v>
@@ -2439,8 +1966,8 @@
       <c r="D38">
         <v>939541443</v>
       </c>
-      <c r="F38" s="2">
-        <v>46021.875</v>
+      <c r="F38" t="s">
+        <v>29</v>
       </c>
       <c r="G38">
         <v>165</v>
@@ -2455,36 +1982,36 @@
         <v>21</v>
       </c>
       <c r="L38" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="1">
-        <v>45391.619378067131</v>
+        <v>30</v>
+      </c>
+      <c r="M38" t="s">
+        <v>31</v>
       </c>
       <c r="N38" t="s">
-        <v>28</v>
-      </c>
-      <c r="O38" s="1">
-        <v>45512.258102442131</v>
+        <v>30</v>
+      </c>
+      <c r="O38" t="s">
+        <v>32</v>
       </c>
       <c r="P38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
         <v>29</v>
-      </c>
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="2">
-        <v>46021.875</v>
       </c>
       <c r="G39">
         <v>327</v>
@@ -2499,36 +2026,36 @@
         <v>21</v>
       </c>
       <c r="L39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="1">
-        <v>45391.618036296299</v>
+        <v>30</v>
+      </c>
+      <c r="M39" t="s">
+        <v>36</v>
       </c>
       <c r="N39" t="s">
-        <v>28</v>
-      </c>
-      <c r="O39" s="1">
-        <v>45512.258493587964</v>
+        <v>30</v>
+      </c>
+      <c r="O39" t="s">
+        <v>37</v>
       </c>
       <c r="P39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="2">
-        <v>46021.875</v>
+        <v>40</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
       </c>
       <c r="G40">
         <v>736</v>
@@ -2543,27 +2070,27 @@
         <v>21</v>
       </c>
       <c r="L40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" t="s">
+        <v>41</v>
+      </c>
+      <c r="N40" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
         <v>28</v>
-      </c>
-      <c r="M40" s="1">
-        <v>45391.616579016205</v>
-      </c>
-      <c r="N40" t="s">
-        <v>28</v>
-      </c>
-      <c r="O40" s="1">
-        <v>45512.258704363427</v>
-      </c>
-      <c r="P40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" t="s">
-        <v>27</v>
       </c>
       <c r="C41">
         <v>939651125</v>
@@ -2571,14 +2098,14 @@
       <c r="D41">
         <v>939651125</v>
       </c>
-      <c r="F41" s="2">
-        <v>46021.875</v>
+      <c r="F41" t="s">
+        <v>29</v>
       </c>
       <c r="G41">
         <v>165</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I41">
         <v>10040</v>
@@ -2587,42 +2114,42 @@
         <v>21</v>
       </c>
       <c r="L41" t="s">
-        <v>28</v>
-      </c>
-      <c r="M41" s="1">
-        <v>45512.299187118057</v>
+        <v>30</v>
+      </c>
+      <c r="M41" t="s">
+        <v>45</v>
       </c>
       <c r="N41" t="s">
-        <v>28</v>
-      </c>
-      <c r="O41" s="1">
-        <v>45512.29930515046</v>
+        <v>30</v>
+      </c>
+      <c r="O41" t="s">
+        <v>46</v>
       </c>
       <c r="P41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="2">
-        <v>46021.875</v>
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
       </c>
       <c r="G42">
         <v>327</v>
       </c>
       <c r="H42" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I42">
         <v>10040</v>
@@ -2631,22 +2158,80 @@
         <v>21</v>
       </c>
       <c r="L42" t="s">
-        <v>28</v>
-      </c>
-      <c r="M42" s="1">
-        <v>45512.328487777777</v>
+        <v>30</v>
+      </c>
+      <c r="M42" t="s">
+        <v>49</v>
       </c>
       <c r="N42" t="s">
-        <v>28</v>
-      </c>
-      <c r="O42" s="1">
-        <v>45512.328574155094</v>
+        <v>30</v>
+      </c>
+      <c r="O42" t="s">
+        <v>50</v>
       </c>
       <c r="P42" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43">
+        <v>1234567</v>
+      </c>
+      <c r="E43">
+        <v>876543211234</v>
+      </c>
+      <c r="F43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43">
+        <v>165</v>
+      </c>
+      <c r="H43" t="s">
+        <v>44</v>
+      </c>
+      <c r="I43">
+        <v>10040</v>
+      </c>
+      <c r="K43" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" t="s">
+        <v>55</v>
+      </c>
+      <c r="N43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" t="s">
+        <v>56</v>
+      </c>
+      <c r="P43" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated master tables data (#4)
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/device_master.xlsx
+++ b/mosip_master/xlsx/device_master.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicholas\Desktop\NIRA MASTERDATA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8655141A-1F73-4947-87DD-E2C23B37D328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C858CEA3-174C-4A7C-B1ED-AE78AACE540F}"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="device_master" sheetId="1" r:id="rId1"/>
+    <sheet name="Worksheet" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -85,13 +80,16 @@
     <t>eng</t>
   </si>
   <si>
-    <t>t</t>
+    <t>true</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>f</t>
+    <t>2024-02-15 06:37:20.005</t>
+  </si>
+  <si>
+    <t>false</t>
   </si>
   <si>
     <t>Mock FingerPrint Scanner</t>
@@ -106,9 +104,18 @@
     <t>RealScan-G10</t>
   </si>
   <si>
+    <t>2025-12-30 21:00:00.000</t>
+  </si>
+  <si>
     <t>globaladmin</t>
   </si>
   <si>
+    <t>2024-04-09 14:51:54.264</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:11:40.050</t>
+  </si>
+  <si>
     <t>a8bcbb3a-93b3-41db-a6d7-0294618fb833</t>
   </si>
   <si>
@@ -118,6 +125,12 @@
     <t>DF0052000024031A</t>
   </si>
   <si>
+    <t>2024-04-09 14:49:58.336</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:12:13.846</t>
+  </si>
+  <si>
     <t>59c43c89-ff00-4041-a933-6d9603e1c331</t>
   </si>
   <si>
@@ -127,558 +140,97 @@
     <t>1FE4516</t>
   </si>
   <si>
+    <t>2024-04-09 14:47:52.426</t>
+  </si>
+  <si>
+    <t>2024-08-08 06:12:32.057</t>
+  </si>
+  <si>
     <t>807b28a8-80cd-47e7-9258-71be5b81f0de</t>
   </si>
   <si>
     <t>UGA</t>
   </si>
   <si>
+    <t>2024-08-08 07:10:49.767</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:10:59.964</t>
+  </si>
+  <si>
     <t>ec48fb6e-1916-4124-bf4a-02f3bbb2f5d1</t>
   </si>
   <si>
     <t>DF0052000020940A</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:53:01.343</t>
+  </si>
+  <si>
+    <t>2024-08-08 07:53:08.806</t>
+  </si>
+  <si>
+    <t>7f8de61a-3e80-42bd-9bf9-374049606439</t>
+  </si>
+  <si>
+    <t>TECHNO-531</t>
+  </si>
+  <si>
+    <t>srbgrb</t>
+  </si>
+  <si>
+    <t>2047-12-30 18:30:00.000</t>
+  </si>
+  <si>
+    <t>2024-08-29 12:42:17.042</t>
+  </si>
+  <si>
+    <t>2024-08-29 12:43:02.606</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Display"/>
-      <family val="2"/>
-      <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
+      <patternFill patternType="gray125">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
+  <borders count="1">
+    <border/>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotTableStyle1"/>
 </styleSheet>
 </file>
 
@@ -693,44 +245,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -758,31 +310,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -810,23 +345,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -838,174 +356,183 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr"/>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EED699B-FD57-42DC-9B0A-D82EBD2217AF}">
-  <dimension ref="A1:Q42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1058,7 +585,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1001</v>
       </c>
@@ -1089,14 +616,14 @@
       <c r="L2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="1">
-        <v>45337.275925995367</v>
+      <c r="M2" t="s">
+        <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>1002</v>
       </c>
@@ -1127,14 +654,14 @@
       <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1">
-        <v>45337.275925995367</v>
+      <c r="M3" t="s">
+        <v>23</v>
       </c>
       <c r="P3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>1003</v>
       </c>
@@ -1165,14 +692,14 @@
       <c r="L4" t="s">
         <v>22</v>
       </c>
-      <c r="M4" s="1">
-        <v>45337.275925995367</v>
+      <c r="M4" t="s">
+        <v>23</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>1004</v>
       </c>
@@ -1203,14 +730,14 @@
       <c r="L5" t="s">
         <v>22</v>
       </c>
-      <c r="M5" s="1">
-        <v>45337.275925995367</v>
+      <c r="M5" t="s">
+        <v>23</v>
       </c>
       <c r="P5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>1005</v>
       </c>
@@ -1241,14 +768,14 @@
       <c r="L6" t="s">
         <v>22</v>
       </c>
-      <c r="M6" s="1">
-        <v>45337.275925995367</v>
+      <c r="M6" t="s">
+        <v>23</v>
       </c>
       <c r="P6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>1006</v>
       </c>
@@ -1279,14 +806,14 @@
       <c r="L7" t="s">
         <v>22</v>
       </c>
-      <c r="M7" s="1">
-        <v>45337.275925995367</v>
+      <c r="M7" t="s">
+        <v>23</v>
       </c>
       <c r="P7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>1007</v>
       </c>
@@ -1317,14 +844,14 @@
       <c r="L8" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="1">
-        <v>45337.275925995367</v>
+      <c r="M8" t="s">
+        <v>23</v>
       </c>
       <c r="P8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>1008</v>
       </c>
@@ -1355,14 +882,14 @@
       <c r="L9" t="s">
         <v>22</v>
       </c>
-      <c r="M9" s="1">
-        <v>45337.275925995367</v>
+      <c r="M9" t="s">
+        <v>23</v>
       </c>
       <c r="P9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>1009</v>
       </c>
@@ -1393,14 +920,14 @@
       <c r="L10" t="s">
         <v>22</v>
       </c>
-      <c r="M10" s="1">
-        <v>45337.275925995367</v>
+      <c r="M10" t="s">
+        <v>23</v>
       </c>
       <c r="P10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>1010</v>
       </c>
@@ -1431,14 +958,14 @@
       <c r="L11" t="s">
         <v>22</v>
       </c>
-      <c r="M11" s="1">
-        <v>45337.275925995367</v>
+      <c r="M11" t="s">
+        <v>23</v>
       </c>
       <c r="P11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>1011</v>
       </c>
@@ -1469,14 +996,14 @@
       <c r="L12" t="s">
         <v>22</v>
       </c>
-      <c r="M12" s="1">
-        <v>45337.275925995367</v>
+      <c r="M12" t="s">
+        <v>23</v>
       </c>
       <c r="P12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13">
         <v>1012</v>
       </c>
@@ -1507,19 +1034,19 @@
       <c r="L13" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="1">
-        <v>45337.275925995367</v>
+      <c r="M13" t="s">
+        <v>23</v>
       </c>
       <c r="P13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14">
         <v>2001</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>18</v>
@@ -1545,19 +1072,19 @@
       <c r="L14" t="s">
         <v>22</v>
       </c>
-      <c r="M14" s="1">
-        <v>45337.275925995367</v>
+      <c r="M14" t="s">
+        <v>23</v>
       </c>
       <c r="P14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15">
         <v>2002</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>18</v>
@@ -1583,19 +1110,19 @@
       <c r="L15" t="s">
         <v>22</v>
       </c>
-      <c r="M15" s="1">
-        <v>45337.275925995367</v>
+      <c r="M15" t="s">
+        <v>23</v>
       </c>
       <c r="P15" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16">
         <v>2003</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
@@ -1621,19 +1148,19 @@
       <c r="L16" t="s">
         <v>22</v>
       </c>
-      <c r="M16" s="1">
-        <v>45337.275925995367</v>
+      <c r="M16" t="s">
+        <v>23</v>
       </c>
       <c r="P16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>2004</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>18</v>
@@ -1659,19 +1186,19 @@
       <c r="L17" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="1">
-        <v>45337.275925995367</v>
+      <c r="M17" t="s">
+        <v>23</v>
       </c>
       <c r="P17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>2005</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>18</v>
@@ -1697,19 +1224,19 @@
       <c r="L18" t="s">
         <v>22</v>
       </c>
-      <c r="M18" s="1">
-        <v>45337.275925995367</v>
+      <c r="M18" t="s">
+        <v>23</v>
       </c>
       <c r="P18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>2006</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>18</v>
@@ -1735,19 +1262,19 @@
       <c r="L19" t="s">
         <v>22</v>
       </c>
-      <c r="M19" s="1">
-        <v>45337.275925995367</v>
+      <c r="M19" t="s">
+        <v>23</v>
       </c>
       <c r="P19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>2007</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>18</v>
@@ -1773,19 +1300,19 @@
       <c r="L20" t="s">
         <v>22</v>
       </c>
-      <c r="M20" s="1">
-        <v>45337.275925995367</v>
+      <c r="M20" t="s">
+        <v>23</v>
       </c>
       <c r="P20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>2008</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>18</v>
@@ -1811,19 +1338,19 @@
       <c r="L21" t="s">
         <v>22</v>
       </c>
-      <c r="M21" s="1">
-        <v>45337.275925995367</v>
+      <c r="M21" t="s">
+        <v>23</v>
       </c>
       <c r="P21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>2009</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>18</v>
@@ -1849,19 +1376,19 @@
       <c r="L22" t="s">
         <v>22</v>
       </c>
-      <c r="M22" s="1">
-        <v>45337.275925995367</v>
+      <c r="M22" t="s">
+        <v>23</v>
       </c>
       <c r="P22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>2010</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>18</v>
@@ -1887,19 +1414,19 @@
       <c r="L23" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="1">
-        <v>45337.275925995367</v>
+      <c r="M23" t="s">
+        <v>23</v>
       </c>
       <c r="P23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>2011</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>18</v>
@@ -1925,19 +1452,19 @@
       <c r="L24" t="s">
         <v>22</v>
       </c>
-      <c r="M24" s="1">
-        <v>45337.275925995367</v>
+      <c r="M24" t="s">
+        <v>23</v>
       </c>
       <c r="P24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>2012</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>18</v>
@@ -1963,19 +1490,19 @@
       <c r="L25" t="s">
         <v>22</v>
       </c>
-      <c r="M25" s="1">
-        <v>45337.275925995367</v>
+      <c r="M25" t="s">
+        <v>23</v>
       </c>
       <c r="P25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>3001</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>18</v>
@@ -2001,19 +1528,19 @@
       <c r="L26" t="s">
         <v>22</v>
       </c>
-      <c r="M26" s="1">
-        <v>45337.275925995367</v>
+      <c r="M26" t="s">
+        <v>23</v>
       </c>
       <c r="P26" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>3002</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
         <v>18</v>
@@ -2039,19 +1566,19 @@
       <c r="L27" t="s">
         <v>22</v>
       </c>
-      <c r="M27" s="1">
-        <v>45337.275925995367</v>
+      <c r="M27" t="s">
+        <v>23</v>
       </c>
       <c r="P27" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>3003</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>18</v>
@@ -2077,19 +1604,19 @@
       <c r="L28" t="s">
         <v>22</v>
       </c>
-      <c r="M28" s="1">
-        <v>45337.275925995367</v>
+      <c r="M28" t="s">
+        <v>23</v>
       </c>
       <c r="P28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>3004</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>18</v>
@@ -2115,19 +1642,19 @@
       <c r="L29" t="s">
         <v>22</v>
       </c>
-      <c r="M29" s="1">
-        <v>45337.275925995367</v>
+      <c r="M29" t="s">
+        <v>23</v>
       </c>
       <c r="P29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>3005</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
         <v>18</v>
@@ -2153,19 +1680,19 @@
       <c r="L30" t="s">
         <v>22</v>
       </c>
-      <c r="M30" s="1">
-        <v>45337.275925995367</v>
+      <c r="M30" t="s">
+        <v>23</v>
       </c>
       <c r="P30" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>3006</v>
       </c>
       <c r="B31" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C31" t="s">
         <v>18</v>
@@ -2191,19 +1718,19 @@
       <c r="L31" t="s">
         <v>22</v>
       </c>
-      <c r="M31" s="1">
-        <v>45337.275925995367</v>
+      <c r="M31" t="s">
+        <v>23</v>
       </c>
       <c r="P31" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>3007</v>
       </c>
       <c r="B32" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C32" t="s">
         <v>18</v>
@@ -2229,19 +1756,19 @@
       <c r="L32" t="s">
         <v>22</v>
       </c>
-      <c r="M32" s="1">
-        <v>45337.275925995367</v>
+      <c r="M32" t="s">
+        <v>23</v>
       </c>
       <c r="P32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>3008</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C33" t="s">
         <v>18</v>
@@ -2267,19 +1794,19 @@
       <c r="L33" t="s">
         <v>22</v>
       </c>
-      <c r="M33" s="1">
-        <v>45337.275925995367</v>
+      <c r="M33" t="s">
+        <v>23</v>
       </c>
       <c r="P33" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>3009</v>
       </c>
       <c r="B34" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
         <v>18</v>
@@ -2305,19 +1832,19 @@
       <c r="L34" t="s">
         <v>22</v>
       </c>
-      <c r="M34" s="1">
-        <v>45337.275925995367</v>
+      <c r="M34" t="s">
+        <v>23</v>
       </c>
       <c r="P34" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>3010</v>
       </c>
       <c r="B35" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
         <v>18</v>
@@ -2343,19 +1870,19 @@
       <c r="L35" t="s">
         <v>22</v>
       </c>
-      <c r="M35" s="1">
-        <v>45337.275925995367</v>
+      <c r="M35" t="s">
+        <v>23</v>
       </c>
       <c r="P35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>3011</v>
       </c>
       <c r="B36" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C36" t="s">
         <v>18</v>
@@ -2381,19 +1908,19 @@
       <c r="L36" t="s">
         <v>22</v>
       </c>
-      <c r="M36" s="1">
-        <v>45337.275925995367</v>
+      <c r="M36" t="s">
+        <v>23</v>
       </c>
       <c r="P36" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>3012</v>
       </c>
       <c r="B37" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C37" t="s">
         <v>18</v>
@@ -2419,19 +1946,19 @@
       <c r="L37" t="s">
         <v>22</v>
       </c>
-      <c r="M37" s="1">
-        <v>45337.275925995367</v>
+      <c r="M37" t="s">
+        <v>23</v>
       </c>
       <c r="P37" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C38">
         <v>939541443</v>
@@ -2439,8 +1966,8 @@
       <c r="D38">
         <v>939541443</v>
       </c>
-      <c r="F38" s="2">
-        <v>46021.875</v>
+      <c r="F38" t="s">
+        <v>29</v>
       </c>
       <c r="G38">
         <v>165</v>
@@ -2455,36 +1982,36 @@
         <v>21</v>
       </c>
       <c r="L38" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="1">
-        <v>45391.619378067131</v>
+        <v>30</v>
+      </c>
+      <c r="M38" t="s">
+        <v>31</v>
       </c>
       <c r="N38" t="s">
-        <v>28</v>
-      </c>
-      <c r="O38" s="1">
-        <v>45512.258102442131</v>
+        <v>30</v>
+      </c>
+      <c r="O38" t="s">
+        <v>32</v>
       </c>
       <c r="P38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F39" t="s">
         <v>29</v>
-      </c>
-      <c r="B39" t="s">
-        <v>30</v>
-      </c>
-      <c r="C39" t="s">
-        <v>31</v>
-      </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="F39" s="2">
-        <v>46021.875</v>
       </c>
       <c r="G39">
         <v>327</v>
@@ -2499,36 +2026,36 @@
         <v>21</v>
       </c>
       <c r="L39" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="1">
-        <v>45391.618036296299</v>
+        <v>30</v>
+      </c>
+      <c r="M39" t="s">
+        <v>36</v>
       </c>
       <c r="N39" t="s">
-        <v>28</v>
-      </c>
-      <c r="O39" s="1">
-        <v>45512.258493587964</v>
+        <v>30</v>
+      </c>
+      <c r="O39" t="s">
+        <v>37</v>
       </c>
       <c r="P39" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>34</v>
-      </c>
-      <c r="F40" s="2">
-        <v>46021.875</v>
+        <v>40</v>
+      </c>
+      <c r="F40" t="s">
+        <v>29</v>
       </c>
       <c r="G40">
         <v>736</v>
@@ -2543,27 +2070,27 @@
         <v>21</v>
       </c>
       <c r="L40" t="s">
+        <v>30</v>
+      </c>
+      <c r="M40" t="s">
+        <v>41</v>
+      </c>
+      <c r="N40" t="s">
+        <v>30</v>
+      </c>
+      <c r="O40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P40" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" t="s">
         <v>28</v>
-      </c>
-      <c r="M40" s="1">
-        <v>45391.616579016205</v>
-      </c>
-      <c r="N40" t="s">
-        <v>28</v>
-      </c>
-      <c r="O40" s="1">
-        <v>45512.258704363427</v>
-      </c>
-      <c r="P40" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" t="s">
-        <v>27</v>
       </c>
       <c r="C41">
         <v>939651125</v>
@@ -2571,14 +2098,14 @@
       <c r="D41">
         <v>939651125</v>
       </c>
-      <c r="F41" s="2">
-        <v>46021.875</v>
+      <c r="F41" t="s">
+        <v>29</v>
       </c>
       <c r="G41">
         <v>165</v>
       </c>
       <c r="H41" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I41">
         <v>10040</v>
@@ -2587,42 +2114,42 @@
         <v>21</v>
       </c>
       <c r="L41" t="s">
-        <v>28</v>
-      </c>
-      <c r="M41" s="1">
-        <v>45512.299187118057</v>
+        <v>30</v>
+      </c>
+      <c r="M41" t="s">
+        <v>45</v>
       </c>
       <c r="N41" t="s">
-        <v>28</v>
-      </c>
-      <c r="O41" s="1">
-        <v>45512.29930515046</v>
+        <v>30</v>
+      </c>
+      <c r="O41" t="s">
+        <v>46</v>
       </c>
       <c r="P41" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B42" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C42" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F42" s="2">
-        <v>46021.875</v>
+        <v>48</v>
+      </c>
+      <c r="F42" t="s">
+        <v>29</v>
       </c>
       <c r="G42">
         <v>327</v>
       </c>
       <c r="H42" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="I42">
         <v>10040</v>
@@ -2631,22 +2158,80 @@
         <v>21</v>
       </c>
       <c r="L42" t="s">
-        <v>28</v>
-      </c>
-      <c r="M42" s="1">
-        <v>45512.328487777777</v>
+        <v>30</v>
+      </c>
+      <c r="M42" t="s">
+        <v>49</v>
       </c>
       <c r="N42" t="s">
-        <v>28</v>
-      </c>
-      <c r="O42" s="1">
-        <v>45512.328574155094</v>
+        <v>30</v>
+      </c>
+      <c r="O42" t="s">
+        <v>50</v>
       </c>
       <c r="P42" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="A43" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" t="s">
+        <v>53</v>
+      </c>
+      <c r="D43">
+        <v>1234567</v>
+      </c>
+      <c r="E43">
+        <v>876543211234</v>
+      </c>
+      <c r="F43" t="s">
+        <v>54</v>
+      </c>
+      <c r="G43">
+        <v>165</v>
+      </c>
+      <c r="H43" t="s">
+        <v>44</v>
+      </c>
+      <c r="I43">
+        <v>10040</v>
+      </c>
+      <c r="K43" t="s">
+        <v>21</v>
+      </c>
+      <c r="L43" t="s">
+        <v>30</v>
+      </c>
+      <c r="M43" t="s">
+        <v>55</v>
+      </c>
+      <c r="N43" t="s">
+        <v>30</v>
+      </c>
+      <c r="O43" t="s">
+        <v>56</v>
+      </c>
+      <c r="P43" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>